<commit_message>
updated out files for dataframes train, valid, and prob
</commit_message>
<xml_diff>
--- a/gen/trainoutput.xlsx
+++ b/gen/trainoutput.xlsx
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1647,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -4045,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="C334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335" spans="1:3">
@@ -4331,7 +4331,7 @@
         <v>1</v>
       </c>
       <c r="C360" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361" spans="1:3">
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="C394" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395" spans="1:3">
@@ -5167,7 +5167,7 @@
         <v>1</v>
       </c>
       <c r="C436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="437" spans="1:3">
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
       <c r="C476" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="477" spans="1:3">
@@ -5706,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="C485" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="486" spans="1:3">
@@ -5992,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="C511" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -6608,7 +6608,7 @@
         <v>1</v>
       </c>
       <c r="C567" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="568" spans="1:3">
@@ -7125,7 +7125,7 @@
         <v>0</v>
       </c>
       <c r="C614" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="615" spans="1:3">
@@ -8401,7 +8401,7 @@
         <v>1</v>
       </c>
       <c r="C730" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:3">
@@ -8610,7 +8610,7 @@
         <v>0</v>
       </c>
       <c r="C749" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="750" spans="1:3">
@@ -9094,7 +9094,7 @@
         <v>0</v>
       </c>
       <c r="C793" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="794" spans="1:3">
@@ -10920,7 +10920,7 @@
         <v>0</v>
       </c>
       <c r="C959" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="960" spans="1:3">
@@ -11536,7 +11536,7 @@
         <v>0</v>
       </c>
       <c r="C1015" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1016" spans="1:3">
@@ -12240,7 +12240,7 @@
         <v>1</v>
       </c>
       <c r="C1079" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1080" spans="1:3">
@@ -12295,7 +12295,7 @@
         <v>0</v>
       </c>
       <c r="C1084" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1085" spans="1:3">
@@ -12383,7 +12383,7 @@
         <v>0</v>
       </c>
       <c r="C1092" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1093" spans="1:3">
@@ -12812,7 +12812,7 @@
         <v>1</v>
       </c>
       <c r="C1131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1132" spans="1:3">
@@ -12933,7 +12933,7 @@
         <v>1</v>
       </c>
       <c r="C1142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1143" spans="1:3">
@@ -14110,7 +14110,7 @@
         <v>0</v>
       </c>
       <c r="C1249" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1250" spans="1:3">
@@ -15738,7 +15738,7 @@
         <v>1</v>
       </c>
       <c r="C1397" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1398" spans="1:3">
@@ -15804,7 +15804,7 @@
         <v>0</v>
       </c>
       <c r="C1403" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1404" spans="1:3">
@@ -16299,7 +16299,7 @@
         <v>0</v>
       </c>
       <c r="C1448" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1449" spans="1:3">
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="C1462" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1463" spans="1:3">
@@ -17553,7 +17553,7 @@
         <v>0</v>
       </c>
       <c r="C1562" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1563" spans="1:3">
@@ -17718,7 +17718,7 @@
         <v>0</v>
       </c>
       <c r="C1577" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1578" spans="1:3">
@@ -17751,7 +17751,7 @@
         <v>0</v>
       </c>
       <c r="C1580" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1581" spans="1:3">
@@ -18587,7 +18587,7 @@
         <v>1</v>
       </c>
       <c r="C1656" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1657" spans="1:3">
@@ -18664,7 +18664,7 @@
         <v>0</v>
       </c>
       <c r="C1663" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1664" spans="1:3">
@@ -19544,7 +19544,7 @@
         <v>1</v>
       </c>
       <c r="C1743" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1744" spans="1:3">
@@ -20952,7 +20952,7 @@
         <v>1</v>
       </c>
       <c r="C1871" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1872" spans="1:3">
@@ -21029,7 +21029,7 @@
         <v>1</v>
       </c>
       <c r="C1878" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1879" spans="1:3">
@@ -21359,7 +21359,7 @@
         <v>1</v>
       </c>
       <c r="C1908" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1909" spans="1:3">

</xml_diff>